<commit_message>
Added updated excel schema notes
</commit_message>
<xml_diff>
--- a/design_notes/foodtrucks_schema.xlsx
+++ b/design_notes/foodtrucks_schema.xlsx
@@ -5,13 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Love Bug\OneDrive\Documents\LambdaProjects-09-20\Oct\unit4\wk4-unit4build-foodtrucktrackr\back-end\design_notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Love Bug\OneDrive\Documents\LambdaProjects-09-20\Oct\unit4\wk4-unit4build-foodtrucktrackr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A710B8-865E-4F02-9B0E-DB040131934D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{65A710B8-865E-4F02-9B0E-DB040131934D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FA215457-04A4-4C1B-8C3B-830C96FC84A8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15930" activeTab="2" xr2:uid="{61D5CFAE-F58D-4A74-BA39-59DDAA551658}"/>
-    <workbookView xWindow="30" yWindow="0" windowWidth="15840" windowHeight="15000" tabRatio="617" xr2:uid="{87E295AE-EF7F-41A9-823C-895342DD7894}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15840" windowHeight="15750" tabRatio="617" xr2:uid="{87E295AE-EF7F-41A9-823C-895342DD7894}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="85">
   <si>
     <t>id</t>
   </si>
@@ -186,9 +185,6 @@
     <t>rating</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>04-menu_items</t>
   </si>
   <si>
@@ -204,12 +200,6 @@
     <t>price</t>
   </si>
   <si>
-    <t>photo</t>
-  </si>
-  <si>
-    <t>customer_id</t>
-  </si>
-  <si>
     <t>menu_item_id</t>
   </si>
   <si>
@@ -286,13 +276,28 @@
   </si>
   <si>
     <t>MENUS</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>photoUrl</t>
+  </si>
+  <si>
+    <t>(optional)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="43" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -498,37 +503,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="7"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="7"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="7"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="2" tint="-0.499984740745262"/>
@@ -586,14 +560,6 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color theme="7"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -619,6 +585,21 @@
       <b/>
       <sz val="18"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -758,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -960,79 +941,58 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1065,31 +1025,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1100,6 +1057,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1414,13 +1386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CAE0017-86EB-4823-B90A-7828916C4FB5}">
-  <dimension ref="A1:W52"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
-    </sheetView>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="1">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1431,28 +1400,30 @@
     <col min="6" max="6" width="16.5" style="6" customWidth="1"/>
     <col min="7" max="7" width="23.1640625" style="6" customWidth="1"/>
     <col min="8" max="8" width="16.5" style="6" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" style="129"/>
-    <col min="10" max="10" width="10.33203125" style="129" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="9.33203125" style="129"/>
+    <col min="9" max="9" width="9.33203125" style="122"/>
+    <col min="10" max="10" width="10.33203125" style="122" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9.33203125" style="122"/>
     <col min="15" max="23" width="9.33203125" style="40"/>
     <col min="24" max="16384" width="9.33203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="17" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="117" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
     </row>
     <row r="2" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
@@ -1475,12 +1446,14 @@
         <v>43</v>
       </c>
       <c r="H2" s="7"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="118" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="17"/>
@@ -1512,12 +1485,14 @@
         <v>8</v>
       </c>
       <c r="H3" s="15"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-      <c r="N3" s="120"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="118" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="113"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="113"/>
+      <c r="N3" s="113"/>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
       <c r="Q3" s="17"/>
@@ -1529,1210 +1504,1382 @@
       <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="106"/>
+      <c r="A4" s="101"/>
       <c r="B4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="114"/>
+      <c r="J4" s="118" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="101"/>
+      <c r="P4" s="101"/>
+      <c r="Q4" s="101"/>
+      <c r="R4" s="101"/>
+      <c r="S4" s="101"/>
+      <c r="T4" s="101"/>
+      <c r="U4" s="101"/>
+      <c r="V4" s="101"/>
+      <c r="W4" s="101"/>
+    </row>
+    <row r="5" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="101"/>
+      <c r="C5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="114"/>
+      <c r="J5" s="114"/>
+      <c r="K5" s="114"/>
+      <c r="L5" s="114"/>
+      <c r="M5" s="114"/>
+      <c r="N5" s="114"/>
+      <c r="O5" s="101"/>
+      <c r="P5" s="101"/>
+      <c r="Q5" s="101"/>
+      <c r="R5" s="101"/>
+      <c r="S5" s="101"/>
+      <c r="T5" s="101"/>
+      <c r="U5" s="101"/>
+      <c r="V5" s="101"/>
+      <c r="W5" s="101"/>
+    </row>
+    <row r="6" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="101"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="114"/>
+      <c r="M6" s="114"/>
+      <c r="N6" s="114"/>
+      <c r="O6" s="101"/>
+      <c r="P6" s="101"/>
+      <c r="Q6" s="101"/>
+      <c r="R6" s="101"/>
+      <c r="S6" s="101"/>
+      <c r="T6" s="101"/>
+      <c r="U6" s="101"/>
+      <c r="V6" s="101"/>
+      <c r="W6" s="101"/>
+    </row>
+    <row r="7" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="101"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114"/>
+      <c r="K7" s="113"/>
+      <c r="L7" s="114"/>
+      <c r="M7" s="114"/>
+      <c r="N7" s="114"/>
+      <c r="O7" s="101"/>
+      <c r="P7" s="101"/>
+      <c r="Q7" s="101"/>
+      <c r="R7" s="101"/>
+      <c r="S7" s="101"/>
+      <c r="T7" s="101"/>
+      <c r="U7" s="101"/>
+      <c r="V7" s="101"/>
+      <c r="W7" s="101"/>
+    </row>
+    <row r="8" spans="1:23" s="18" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="129" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="143"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="115"/>
+      <c r="J8" s="115"/>
+      <c r="K8" s="115"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
+    </row>
+    <row r="9" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="92" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="92" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="92" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="92" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="92"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="115"/>
+      <c r="K9" s="114"/>
+      <c r="L9" s="115"/>
+      <c r="M9" s="115"/>
+      <c r="N9" s="115"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+    </row>
+    <row r="10" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="93"/>
+      <c r="I10" s="115"/>
+      <c r="J10" s="115"/>
+      <c r="K10" s="115"/>
+      <c r="L10" s="115"/>
+      <c r="M10" s="115"/>
+      <c r="N10" s="115"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+    </row>
+    <row r="11" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="103"/>
+      <c r="B11" s="94" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="94" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="94" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="94" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="94"/>
+      <c r="I11" s="116"/>
+      <c r="J11" s="116"/>
+      <c r="K11" s="116"/>
+      <c r="L11" s="116"/>
+      <c r="M11" s="116"/>
+      <c r="N11" s="116"/>
+      <c r="O11" s="103"/>
+      <c r="P11" s="103"/>
+      <c r="Q11" s="103"/>
+      <c r="R11" s="103"/>
+      <c r="S11" s="103"/>
+      <c r="T11" s="103"/>
+      <c r="U11" s="103"/>
+      <c r="V11" s="103"/>
+      <c r="W11" s="103"/>
+    </row>
+    <row r="12" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="103"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="94"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="116"/>
+      <c r="L12" s="116"/>
+      <c r="M12" s="116"/>
+      <c r="N12" s="116"/>
+      <c r="O12" s="103"/>
+      <c r="P12" s="103"/>
+      <c r="Q12" s="103"/>
+      <c r="R12" s="103"/>
+      <c r="S12" s="103"/>
+      <c r="T12" s="103"/>
+      <c r="U12" s="103"/>
+      <c r="V12" s="103"/>
+      <c r="W12" s="103"/>
+    </row>
+    <row r="13" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="103"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="116"/>
+      <c r="J13" s="116"/>
+      <c r="K13" s="116"/>
+      <c r="L13" s="116"/>
+      <c r="M13" s="116"/>
+      <c r="N13" s="116"/>
+      <c r="O13" s="103"/>
+      <c r="P13" s="103"/>
+      <c r="Q13" s="103"/>
+      <c r="R13" s="103"/>
+      <c r="S13" s="103"/>
+      <c r="T13" s="103"/>
+      <c r="U13" s="103"/>
+      <c r="V13" s="103"/>
+      <c r="W13" s="103"/>
+    </row>
+    <row r="14" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="103"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="116"/>
+      <c r="J14" s="116"/>
+      <c r="K14" s="114"/>
+      <c r="L14" s="116"/>
+      <c r="M14" s="116"/>
+      <c r="N14" s="116"/>
+      <c r="O14" s="103"/>
+      <c r="P14" s="103"/>
+      <c r="Q14" s="103"/>
+      <c r="R14" s="103"/>
+      <c r="S14" s="103"/>
+      <c r="T14" s="103"/>
+      <c r="U14" s="103"/>
+      <c r="V14" s="103"/>
+      <c r="W14" s="103"/>
+    </row>
+    <row r="15" spans="1:23" s="19" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="128" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="104"/>
+      <c r="G15" s="104"/>
+      <c r="H15" s="104"/>
+      <c r="I15" s="117"/>
+      <c r="J15" s="117"/>
+      <c r="K15" s="117"/>
+      <c r="L15" s="117"/>
+      <c r="M15" s="117"/>
+      <c r="N15" s="117"/>
+    </row>
+    <row r="16" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="117"/>
+      <c r="J16" s="117"/>
+      <c r="K16" s="117"/>
+      <c r="L16" s="117"/>
+      <c r="M16" s="117"/>
+      <c r="N16" s="117"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="19"/>
+    </row>
+    <row r="17" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="117"/>
+      <c r="J17" s="117"/>
+      <c r="K17" s="117"/>
+      <c r="L17" s="117"/>
+      <c r="M17" s="117"/>
+      <c r="N17" s="117"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+    </row>
+    <row r="18" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="95"/>
+      <c r="B18" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="95"/>
+      <c r="K18" s="118"/>
+      <c r="L18" s="118"/>
+      <c r="M18" s="118"/>
+      <c r="N18" s="118"/>
+      <c r="O18" s="95"/>
+      <c r="P18" s="95"/>
+      <c r="Q18" s="95"/>
+      <c r="R18" s="95"/>
+      <c r="S18" s="95"/>
+      <c r="T18" s="95"/>
+      <c r="U18" s="95"/>
+      <c r="V18" s="95"/>
+      <c r="W18" s="95"/>
+    </row>
+    <row r="19" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="95"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="118"/>
+      <c r="J19" s="95"/>
+      <c r="K19" s="118"/>
+      <c r="L19" s="118"/>
+      <c r="M19" s="118"/>
+      <c r="N19" s="118"/>
+      <c r="O19" s="95"/>
+      <c r="P19" s="95"/>
+      <c r="Q19" s="95"/>
+      <c r="R19" s="95"/>
+      <c r="S19" s="95"/>
+      <c r="T19" s="95"/>
+      <c r="U19" s="95"/>
+      <c r="V19" s="95"/>
+      <c r="W19" s="95"/>
+    </row>
+    <row r="20" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="95"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="118"/>
+      <c r="J20" s="95"/>
+      <c r="K20" s="118"/>
+      <c r="L20" s="118"/>
+      <c r="M20" s="118"/>
+      <c r="N20" s="118"/>
+      <c r="O20" s="95"/>
+      <c r="P20" s="95"/>
+      <c r="Q20" s="95"/>
+      <c r="R20" s="95"/>
+      <c r="S20" s="95"/>
+      <c r="T20" s="95"/>
+      <c r="U20" s="95"/>
+      <c r="V20" s="95"/>
+      <c r="W20" s="95"/>
+    </row>
+    <row r="21" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="95"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="118"/>
+      <c r="J21" s="95"/>
+      <c r="K21" s="118"/>
+      <c r="L21" s="118"/>
+      <c r="M21" s="118"/>
+      <c r="N21" s="118"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="95"/>
+      <c r="R21" s="95"/>
+      <c r="S21" s="95"/>
+      <c r="T21" s="95"/>
+      <c r="U21" s="95"/>
+      <c r="V21" s="95"/>
+      <c r="W21" s="95"/>
+    </row>
+    <row r="22" spans="1:23" s="20" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="127" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="119"/>
+      <c r="J22" s="119"/>
+      <c r="K22" s="119"/>
+      <c r="L22" s="119"/>
+      <c r="M22" s="119"/>
+      <c r="N22" s="119"/>
+    </row>
+    <row r="23" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="119"/>
+      <c r="J23" s="119"/>
+      <c r="K23" s="119"/>
+      <c r="L23" s="119"/>
+      <c r="M23" s="119"/>
+      <c r="N23" s="119"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="20"/>
+    </row>
+    <row r="24" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="119"/>
+      <c r="J24" s="119"/>
+      <c r="K24" s="119"/>
+      <c r="L24" s="119"/>
+      <c r="M24" s="119"/>
+      <c r="N24" s="119"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="20"/>
+      <c r="U24" s="20"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="20"/>
+    </row>
+    <row r="25" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="106"/>
+      <c r="B25" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="120"/>
+      <c r="J25" s="120"/>
+      <c r="K25" s="120"/>
+      <c r="L25" s="120"/>
+      <c r="M25" s="120"/>
+      <c r="N25" s="120"/>
+      <c r="O25" s="106"/>
+      <c r="P25" s="106"/>
+      <c r="Q25" s="106"/>
+      <c r="R25" s="106"/>
+      <c r="S25" s="106"/>
+      <c r="T25" s="106"/>
+      <c r="U25" s="106"/>
+      <c r="V25" s="106"/>
+      <c r="W25" s="106"/>
+    </row>
+    <row r="26" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="106"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="120"/>
+      <c r="J26" s="120"/>
+      <c r="K26" s="120"/>
+      <c r="L26" s="120"/>
+      <c r="M26" s="120"/>
+      <c r="N26" s="120"/>
+      <c r="O26" s="106"/>
+      <c r="P26" s="106"/>
+      <c r="Q26" s="106"/>
+      <c r="R26" s="106"/>
+      <c r="S26" s="106"/>
+      <c r="T26" s="106"/>
+      <c r="U26" s="106"/>
+      <c r="V26" s="106"/>
+      <c r="W26" s="106"/>
+    </row>
+    <row r="27" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="106"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="120"/>
+      <c r="J27" s="120"/>
+      <c r="K27" s="120"/>
+      <c r="L27" s="120"/>
+      <c r="M27" s="120"/>
+      <c r="N27" s="120"/>
+      <c r="O27" s="106"/>
+      <c r="P27" s="106"/>
+      <c r="Q27" s="106"/>
+      <c r="R27" s="106"/>
+      <c r="S27" s="106"/>
+      <c r="T27" s="106"/>
+      <c r="U27" s="106"/>
+      <c r="V27" s="106"/>
+      <c r="W27" s="106"/>
+    </row>
+    <row r="28" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="106"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="120"/>
+      <c r="J28" s="120"/>
+      <c r="K28" s="120"/>
+      <c r="L28" s="120"/>
+      <c r="M28" s="120"/>
+      <c r="N28" s="120"/>
+      <c r="O28" s="106"/>
+      <c r="P28" s="106"/>
+      <c r="Q28" s="106"/>
+      <c r="R28" s="106"/>
+      <c r="S28" s="106"/>
+      <c r="T28" s="106"/>
+      <c r="U28" s="106"/>
+      <c r="V28" s="106"/>
+      <c r="W28" s="106"/>
+    </row>
+    <row r="29" spans="1:23" s="20" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="126" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="121"/>
-      <c r="J4" s="121"/>
-      <c r="K4" s="121"/>
-      <c r="L4" s="121"/>
-      <c r="M4" s="121"/>
-      <c r="N4" s="121"/>
-      <c r="O4" s="106"/>
-      <c r="P4" s="106"/>
-      <c r="Q4" s="106"/>
-      <c r="R4" s="106"/>
-      <c r="S4" s="106"/>
-      <c r="T4" s="106"/>
-      <c r="U4" s="106"/>
-      <c r="V4" s="106"/>
-      <c r="W4" s="106"/>
-    </row>
-    <row r="5" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="106"/>
-      <c r="I5" s="121"/>
-      <c r="J5" s="121"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="121"/>
-      <c r="M5" s="121"/>
-      <c r="N5" s="121"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="106"/>
-    </row>
-    <row r="6" spans="1:23" s="18" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="137" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="107"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="122"/>
-      <c r="J6" s="122"/>
-      <c r="K6" s="122"/>
-      <c r="L6" s="121"/>
-      <c r="M6" s="121"/>
-      <c r="N6" s="122"/>
-    </row>
-    <row r="7" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="92" t="s">
+      <c r="C29" s="140"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="108"/>
+      <c r="F29" s="108"/>
+      <c r="G29" s="108"/>
+      <c r="H29" s="108"/>
+      <c r="I29" s="119"/>
+      <c r="J29" s="119"/>
+      <c r="K29" s="119"/>
+      <c r="L29" s="119"/>
+      <c r="M29" s="119"/>
+      <c r="N29" s="119"/>
+    </row>
+    <row r="30" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
+      <c r="B30" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="92" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="92" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="92" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="92"/>
-      <c r="I7" s="122"/>
-      <c r="J7" s="122"/>
-      <c r="K7" s="121"/>
-      <c r="L7" s="122"/>
-      <c r="M7" s="122"/>
-      <c r="N7" s="122"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-    </row>
-    <row r="8" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="93" t="s">
+      <c r="C30" s="92" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="96" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="96" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" s="96"/>
+      <c r="H30" s="96"/>
+      <c r="I30" s="119"/>
+      <c r="J30" s="119"/>
+      <c r="K30" s="119"/>
+      <c r="L30" s="119"/>
+      <c r="M30" s="119"/>
+      <c r="N30" s="119"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="20"/>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="20"/>
+      <c r="S30" s="20"/>
+      <c r="T30" s="20"/>
+      <c r="U30" s="20"/>
+      <c r="V30" s="20"/>
+      <c r="W30" s="20"/>
+    </row>
+    <row r="31" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
+      <c r="B31" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="93" t="s">
+      <c r="C31" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="97" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="93" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="93" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="93" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="93" t="s">
+      <c r="G31" s="97"/>
+      <c r="H31" s="97"/>
+      <c r="I31" s="119"/>
+      <c r="J31" s="119"/>
+      <c r="K31" s="119"/>
+      <c r="L31" s="119"/>
+      <c r="M31" s="119"/>
+      <c r="N31" s="119"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="20"/>
+      <c r="S31" s="20"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="20"/>
+      <c r="V31" s="20"/>
+      <c r="W31" s="20"/>
+    </row>
+    <row r="32" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="106"/>
+      <c r="B32" s="98" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="94" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="109" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="98" t="s">
+        <v>84</v>
+      </c>
+      <c r="G32" s="98"/>
+      <c r="H32" s="98"/>
+      <c r="I32" s="120"/>
+      <c r="J32" s="120"/>
+      <c r="K32" s="120"/>
+      <c r="L32" s="120"/>
+      <c r="M32" s="120"/>
+      <c r="N32" s="120"/>
+      <c r="O32" s="106"/>
+      <c r="P32" s="106"/>
+      <c r="Q32" s="106"/>
+      <c r="R32" s="106"/>
+      <c r="S32" s="106"/>
+      <c r="T32" s="106"/>
+      <c r="U32" s="106"/>
+      <c r="V32" s="106"/>
+      <c r="W32" s="106"/>
+    </row>
+    <row r="33" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="106"/>
+      <c r="B33" s="98"/>
+      <c r="C33" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="98"/>
+      <c r="F33" s="98"/>
+      <c r="G33" s="98"/>
+      <c r="H33" s="98"/>
+      <c r="I33" s="120"/>
+      <c r="J33" s="120"/>
+      <c r="K33" s="120"/>
+      <c r="L33" s="120"/>
+      <c r="M33" s="120"/>
+      <c r="N33" s="120"/>
+      <c r="O33" s="106"/>
+      <c r="P33" s="106"/>
+      <c r="Q33" s="106"/>
+      <c r="R33" s="106"/>
+      <c r="S33" s="106"/>
+      <c r="T33" s="106"/>
+      <c r="U33" s="106"/>
+      <c r="V33" s="106"/>
+      <c r="W33" s="106"/>
+    </row>
+    <row r="34" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="106"/>
+      <c r="B34" s="98"/>
+      <c r="C34" s="94"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="98"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="120"/>
+      <c r="J34" s="120"/>
+      <c r="K34" s="120"/>
+      <c r="L34" s="120"/>
+      <c r="M34" s="120"/>
+      <c r="N34" s="120"/>
+      <c r="O34" s="106"/>
+      <c r="P34" s="106"/>
+      <c r="Q34" s="106"/>
+      <c r="R34" s="106"/>
+      <c r="S34" s="106"/>
+      <c r="T34" s="106"/>
+      <c r="U34" s="106"/>
+      <c r="V34" s="106"/>
+      <c r="W34" s="106"/>
+    </row>
+    <row r="35" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="106"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="141"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="98"/>
+      <c r="I35" s="120"/>
+      <c r="J35" s="120"/>
+      <c r="K35" s="120"/>
+      <c r="L35" s="120"/>
+      <c r="M35" s="120"/>
+      <c r="N35" s="120"/>
+      <c r="O35" s="106"/>
+      <c r="P35" s="106"/>
+      <c r="Q35" s="106"/>
+      <c r="R35" s="106"/>
+      <c r="S35" s="106"/>
+      <c r="T35" s="106"/>
+      <c r="U35" s="106"/>
+      <c r="V35" s="106"/>
+      <c r="W35" s="106"/>
+    </row>
+    <row r="36" spans="1:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="107"/>
+      <c r="B36" s="99"/>
+      <c r="C36" s="142"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="99"/>
+      <c r="F36" s="99"/>
+      <c r="G36" s="99"/>
+      <c r="H36" s="99"/>
+      <c r="I36" s="121"/>
+      <c r="J36" s="121"/>
+      <c r="K36" s="121"/>
+      <c r="L36" s="121"/>
+      <c r="M36" s="121"/>
+      <c r="N36" s="121"/>
+      <c r="O36" s="107"/>
+      <c r="P36" s="107"/>
+      <c r="Q36" s="107"/>
+      <c r="R36" s="107"/>
+      <c r="S36" s="107"/>
+      <c r="T36" s="107"/>
+      <c r="U36" s="107"/>
+      <c r="V36" s="107"/>
+      <c r="W36" s="107"/>
+    </row>
+    <row r="37" spans="1:23" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="95"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="95"/>
+      <c r="F37" s="95"/>
+      <c r="G37" s="95"/>
+      <c r="H37" s="95"/>
+      <c r="I37" s="122"/>
+      <c r="J37" s="122"/>
+      <c r="K37" s="122"/>
+      <c r="L37" s="122"/>
+      <c r="M37" s="122"/>
+      <c r="N37" s="122"/>
+    </row>
+    <row r="38" spans="1:23" s="20" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="126" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="108"/>
+      <c r="E38" s="108"/>
+      <c r="F38" s="108"/>
+      <c r="G38" s="108"/>
+      <c r="H38" s="108"/>
+      <c r="I38" s="123"/>
+      <c r="J38" s="119"/>
+      <c r="K38" s="119"/>
+      <c r="L38" s="119"/>
+      <c r="M38" s="119"/>
+      <c r="N38" s="119"/>
+    </row>
+    <row r="39" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="20"/>
+      <c r="B39" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="96"/>
+      <c r="F39" s="96"/>
+      <c r="G39" s="96"/>
+      <c r="H39" s="96"/>
+      <c r="I39" s="123"/>
+      <c r="J39" s="119"/>
+      <c r="K39" s="119"/>
+      <c r="L39" s="119"/>
+      <c r="M39" s="119"/>
+      <c r="N39" s="119"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="20"/>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="20"/>
+      <c r="T39" s="20"/>
+      <c r="U39" s="20"/>
+      <c r="V39" s="20"/>
+      <c r="W39" s="20"/>
+    </row>
+    <row r="40" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="20"/>
+      <c r="B40" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="93"/>
-      <c r="I8" s="122"/>
-      <c r="J8" s="122"/>
-      <c r="K8" s="122"/>
-      <c r="L8" s="122"/>
-      <c r="M8" s="122"/>
-      <c r="N8" s="122"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-    </row>
-    <row r="9" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="108"/>
-      <c r="B9" s="94" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="123"/>
-      <c r="M9" s="123"/>
-      <c r="N9" s="123"/>
-      <c r="O9" s="108"/>
-      <c r="P9" s="108"/>
-      <c r="Q9" s="108"/>
-      <c r="R9" s="108"/>
-      <c r="S9" s="108"/>
-      <c r="T9" s="108"/>
-      <c r="U9" s="108"/>
-      <c r="V9" s="108"/>
-      <c r="W9" s="108"/>
-    </row>
-    <row r="10" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="108"/>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="123"/>
-      <c r="J10" s="123"/>
-      <c r="K10" s="121"/>
-      <c r="L10" s="123"/>
-      <c r="M10" s="123"/>
-      <c r="N10" s="123"/>
-      <c r="O10" s="108"/>
-      <c r="P10" s="108"/>
-      <c r="Q10" s="108"/>
-      <c r="R10" s="108"/>
-      <c r="S10" s="108"/>
-      <c r="T10" s="108"/>
-      <c r="U10" s="108"/>
-      <c r="V10" s="108"/>
-      <c r="W10" s="108"/>
-    </row>
-    <row r="11" spans="1:23" s="19" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="136" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="109"/>
-      <c r="E11" s="109"/>
-      <c r="F11" s="109"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="124"/>
-      <c r="J11" s="124"/>
-      <c r="K11" s="124"/>
-      <c r="L11" s="124"/>
-      <c r="M11" s="124"/>
-      <c r="N11" s="124"/>
-    </row>
-    <row r="12" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="8" t="s">
+      <c r="C40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="97"/>
+      <c r="F40" s="97"/>
+      <c r="G40" s="97"/>
+      <c r="H40" s="97"/>
+      <c r="I40" s="123"/>
+      <c r="J40" s="119"/>
+      <c r="K40" s="119"/>
+      <c r="L40" s="119"/>
+      <c r="M40" s="119"/>
+      <c r="N40" s="119"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="20"/>
+      <c r="T40" s="20"/>
+      <c r="U40" s="20"/>
+      <c r="V40" s="20"/>
+      <c r="W40" s="20"/>
+    </row>
+    <row r="41" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="106"/>
+      <c r="B41" s="98" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="109"/>
+      <c r="F41" s="98"/>
+      <c r="G41" s="98"/>
+      <c r="H41" s="98"/>
+      <c r="I41" s="124"/>
+      <c r="J41" s="120"/>
+      <c r="K41" s="120"/>
+      <c r="L41" s="120"/>
+      <c r="M41" s="120"/>
+      <c r="N41" s="120"/>
+      <c r="O41" s="106"/>
+      <c r="P41" s="106"/>
+      <c r="Q41" s="106"/>
+      <c r="R41" s="106"/>
+      <c r="S41" s="106"/>
+      <c r="T41" s="106"/>
+      <c r="U41" s="106"/>
+      <c r="V41" s="106"/>
+      <c r="W41" s="106"/>
+    </row>
+    <row r="42" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="106"/>
+      <c r="B42" s="98"/>
+      <c r="C42" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="98"/>
+      <c r="F42" s="98"/>
+      <c r="G42" s="98"/>
+      <c r="H42" s="98"/>
+      <c r="I42" s="124"/>
+      <c r="J42" s="120"/>
+      <c r="K42" s="120"/>
+      <c r="L42" s="120"/>
+      <c r="M42" s="120"/>
+      <c r="N42" s="120"/>
+      <c r="O42" s="106"/>
+      <c r="P42" s="106"/>
+      <c r="Q42" s="106"/>
+      <c r="R42" s="106"/>
+      <c r="S42" s="106"/>
+      <c r="T42" s="106"/>
+      <c r="U42" s="106"/>
+      <c r="V42" s="106"/>
+      <c r="W42" s="106"/>
+    </row>
+    <row r="43" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="106"/>
+      <c r="B43" s="98"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="98"/>
+      <c r="F43" s="98"/>
+      <c r="G43" s="98"/>
+      <c r="H43" s="98"/>
+      <c r="I43" s="124"/>
+      <c r="J43" s="120"/>
+      <c r="K43" s="120"/>
+      <c r="L43" s="120"/>
+      <c r="M43" s="120"/>
+      <c r="N43" s="120"/>
+      <c r="O43" s="106"/>
+      <c r="P43" s="106"/>
+      <c r="Q43" s="106"/>
+      <c r="R43" s="106"/>
+      <c r="S43" s="106"/>
+      <c r="T43" s="106"/>
+      <c r="U43" s="106"/>
+      <c r="V43" s="106"/>
+      <c r="W43" s="106"/>
+    </row>
+    <row r="44" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="106"/>
+      <c r="B44" s="98"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="98"/>
+      <c r="F44" s="98"/>
+      <c r="G44" s="98"/>
+      <c r="H44" s="98"/>
+      <c r="I44" s="124"/>
+      <c r="J44" s="120"/>
+      <c r="K44" s="120"/>
+      <c r="L44" s="120"/>
+      <c r="M44" s="120"/>
+      <c r="N44" s="120"/>
+      <c r="O44" s="106"/>
+      <c r="P44" s="106"/>
+      <c r="Q44" s="106"/>
+      <c r="R44" s="106"/>
+      <c r="S44" s="106"/>
+      <c r="T44" s="106"/>
+      <c r="U44" s="106"/>
+      <c r="V44" s="106"/>
+      <c r="W44" s="106"/>
+    </row>
+    <row r="45" spans="1:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="107"/>
+      <c r="B45" s="99"/>
+      <c r="C45" s="110"/>
+      <c r="D45" s="111"/>
+      <c r="E45" s="99"/>
+      <c r="F45" s="99"/>
+      <c r="G45" s="99"/>
+      <c r="H45" s="99"/>
+      <c r="I45" s="125"/>
+      <c r="J45" s="121"/>
+      <c r="K45" s="121"/>
+      <c r="L45" s="121"/>
+      <c r="M45" s="121"/>
+      <c r="N45" s="121"/>
+      <c r="O45" s="107"/>
+      <c r="P45" s="107"/>
+      <c r="Q45" s="107"/>
+      <c r="R45" s="107"/>
+      <c r="S45" s="107"/>
+      <c r="T45" s="107"/>
+      <c r="U45" s="107"/>
+      <c r="V45" s="107"/>
+      <c r="W45" s="107"/>
+    </row>
+    <row r="46" spans="1:23" s="20" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="126" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="143"/>
+      <c r="D46" s="104"/>
+      <c r="E46" s="108"/>
+      <c r="F46" s="108"/>
+      <c r="G46" s="108"/>
+      <c r="H46" s="108"/>
+      <c r="I46" s="123"/>
+      <c r="J46" s="119"/>
+      <c r="K46" s="119"/>
+      <c r="L46" s="119"/>
+      <c r="M46" s="119"/>
+      <c r="N46" s="119"/>
+    </row>
+    <row r="47" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="20"/>
+      <c r="B47" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="124"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="124"/>
-      <c r="L12" s="124"/>
-      <c r="M12" s="124"/>
-      <c r="N12" s="124"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="19"/>
-      <c r="W12" s="19"/>
-    </row>
-    <row r="13" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="16" t="s">
+      <c r="C47" s="92" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E47" s="96"/>
+      <c r="F47" s="96"/>
+      <c r="G47" s="96"/>
+      <c r="H47" s="96"/>
+      <c r="I47" s="123"/>
+      <c r="J47" s="119"/>
+      <c r="K47" s="119"/>
+      <c r="L47" s="119"/>
+      <c r="M47" s="119"/>
+      <c r="N47" s="119"/>
+      <c r="O47" s="20"/>
+      <c r="P47" s="20"/>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="20"/>
+      <c r="S47" s="20"/>
+      <c r="T47" s="20"/>
+      <c r="U47" s="20"/>
+      <c r="V47" s="20"/>
+      <c r="W47" s="20"/>
+    </row>
+    <row r="48" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="20"/>
+      <c r="B48" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="16" t="s">
+      <c r="C48" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="124"/>
-      <c r="J13" s="124"/>
-      <c r="K13" s="124"/>
-      <c r="L13" s="124"/>
-      <c r="M13" s="124"/>
-      <c r="N13" s="124"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="19"/>
-    </row>
-    <row r="14" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="96"/>
-      <c r="B14" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="125"/>
-      <c r="J14" s="124" t="s">
-        <v>62</v>
-      </c>
-      <c r="K14" s="125"/>
-      <c r="L14" s="125"/>
-      <c r="M14" s="125"/>
-      <c r="N14" s="125"/>
-      <c r="O14" s="96"/>
-      <c r="P14" s="96"/>
-      <c r="Q14" s="96"/>
-      <c r="R14" s="96"/>
-      <c r="S14" s="96"/>
-      <c r="T14" s="96"/>
-      <c r="U14" s="96"/>
-      <c r="V14" s="96"/>
-      <c r="W14" s="96"/>
-    </row>
-    <row r="15" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="96"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="125"/>
-      <c r="J15" s="125" t="s">
-        <v>63</v>
-      </c>
-      <c r="K15" s="125"/>
-      <c r="L15" s="125"/>
-      <c r="M15" s="125"/>
-      <c r="N15" s="125"/>
-      <c r="O15" s="96"/>
-      <c r="P15" s="96"/>
-      <c r="Q15" s="96"/>
-      <c r="R15" s="96"/>
-      <c r="S15" s="96"/>
-      <c r="T15" s="96"/>
-      <c r="U15" s="96"/>
-      <c r="V15" s="96"/>
-      <c r="W15" s="96"/>
-    </row>
-    <row r="16" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="96"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="125"/>
-      <c r="J16" s="125" t="s">
-        <v>64</v>
-      </c>
-      <c r="K16" s="125"/>
-      <c r="L16" s="125"/>
-      <c r="M16" s="125"/>
-      <c r="N16" s="125"/>
-      <c r="O16" s="96"/>
-      <c r="P16" s="96"/>
-      <c r="Q16" s="96"/>
-      <c r="R16" s="96"/>
-      <c r="S16" s="96"/>
-      <c r="T16" s="96"/>
-      <c r="U16" s="96"/>
-      <c r="V16" s="96"/>
-      <c r="W16" s="96"/>
-    </row>
-    <row r="17" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="96"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="125"/>
-      <c r="J17" s="125" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="125"/>
-      <c r="L17" s="125"/>
-      <c r="M17" s="125"/>
-      <c r="N17" s="125"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="96"/>
-      <c r="S17" s="96"/>
-      <c r="T17" s="96"/>
-      <c r="U17" s="96"/>
-      <c r="V17" s="96"/>
-      <c r="W17" s="96"/>
-    </row>
-    <row r="18" spans="1:23" s="20" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="135" t="s">
+      <c r="D48" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="97"/>
+      <c r="F48" s="97"/>
+      <c r="G48" s="97"/>
+      <c r="H48" s="97"/>
+      <c r="I48" s="123"/>
+      <c r="J48" s="119"/>
+      <c r="K48" s="119"/>
+      <c r="L48" s="119"/>
+      <c r="M48" s="119"/>
+      <c r="N48" s="119"/>
+      <c r="O48" s="20"/>
+      <c r="P48" s="20"/>
+      <c r="Q48" s="20"/>
+      <c r="R48" s="20"/>
+      <c r="S48" s="20"/>
+      <c r="T48" s="20"/>
+      <c r="U48" s="20"/>
+      <c r="V48" s="20"/>
+      <c r="W48" s="20"/>
+    </row>
+    <row r="49" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="106"/>
+      <c r="B49" s="98" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="110"/>
-      <c r="E18" s="110"/>
-      <c r="F18" s="110"/>
-      <c r="G18" s="110"/>
-      <c r="H18" s="110"/>
-      <c r="I18" s="126"/>
-      <c r="J18" s="126"/>
-      <c r="K18" s="126"/>
-      <c r="L18" s="126"/>
-      <c r="M18" s="126"/>
-      <c r="N18" s="126"/>
-    </row>
-    <row r="19" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="126"/>
-      <c r="J19" s="126"/>
-      <c r="K19" s="126"/>
-      <c r="L19" s="126"/>
-      <c r="M19" s="126"/>
-      <c r="N19" s="126"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20"/>
-      <c r="U19" s="20"/>
-      <c r="V19" s="20"/>
-      <c r="W19" s="20"/>
-    </row>
-    <row r="20" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="126"/>
-      <c r="J20" s="126"/>
-      <c r="K20" s="126"/>
-      <c r="L20" s="126"/>
-      <c r="M20" s="126"/>
-      <c r="N20" s="126"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
-      <c r="U20" s="20"/>
-      <c r="V20" s="20"/>
-      <c r="W20" s="20"/>
-    </row>
-    <row r="21" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="111"/>
-      <c r="B21" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="24" t="s">
+      <c r="C49" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="127"/>
-      <c r="J21" s="127"/>
-      <c r="K21" s="127"/>
-      <c r="L21" s="127"/>
-      <c r="M21" s="127"/>
-      <c r="N21" s="127"/>
-      <c r="O21" s="111"/>
-      <c r="P21" s="111"/>
-      <c r="Q21" s="111"/>
-      <c r="R21" s="111"/>
-      <c r="S21" s="111"/>
-      <c r="T21" s="111"/>
-      <c r="U21" s="111"/>
-      <c r="V21" s="111"/>
-      <c r="W21" s="111"/>
-    </row>
-    <row r="22" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="111"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="127"/>
-      <c r="J22" s="127"/>
-      <c r="K22" s="127"/>
-      <c r="L22" s="127"/>
-      <c r="M22" s="127"/>
-      <c r="N22" s="127"/>
-      <c r="O22" s="111"/>
-      <c r="P22" s="111"/>
-      <c r="Q22" s="111"/>
-      <c r="R22" s="111"/>
-      <c r="S22" s="111"/>
-      <c r="T22" s="111"/>
-      <c r="U22" s="111"/>
-      <c r="V22" s="111"/>
-      <c r="W22" s="111"/>
-    </row>
-    <row r="23" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="111"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="127"/>
-      <c r="J23" s="127"/>
-      <c r="K23" s="127"/>
-      <c r="L23" s="127"/>
-      <c r="M23" s="127"/>
-      <c r="N23" s="127"/>
-      <c r="O23" s="111"/>
-      <c r="P23" s="111"/>
-      <c r="Q23" s="111"/>
-      <c r="R23" s="111"/>
-      <c r="S23" s="111"/>
-      <c r="T23" s="111"/>
-      <c r="U23" s="111"/>
-      <c r="V23" s="111"/>
-      <c r="W23" s="111"/>
-    </row>
-    <row r="24" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="111"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="127"/>
-      <c r="J24" s="127"/>
-      <c r="K24" s="127"/>
-      <c r="L24" s="127"/>
-      <c r="M24" s="127"/>
-      <c r="N24" s="127"/>
-      <c r="O24" s="111"/>
-      <c r="P24" s="111"/>
-      <c r="Q24" s="111"/>
-      <c r="R24" s="111"/>
-      <c r="S24" s="111"/>
-      <c r="T24" s="111"/>
-      <c r="U24" s="111"/>
-      <c r="V24" s="111"/>
-      <c r="W24" s="111"/>
-    </row>
-    <row r="25" spans="1:23" s="20" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="134" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="112"/>
-      <c r="E25" s="112"/>
-      <c r="F25" s="112"/>
-      <c r="G25" s="112"/>
-      <c r="H25" s="112"/>
-      <c r="I25" s="126"/>
-      <c r="J25" s="126"/>
-      <c r="K25" s="126"/>
-      <c r="L25" s="126"/>
-      <c r="M25" s="126"/>
-      <c r="N25" s="126"/>
-    </row>
-    <row r="26" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="97" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="97" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="97"/>
-      <c r="G26" s="97"/>
-      <c r="H26" s="97"/>
-      <c r="I26" s="126"/>
-      <c r="J26" s="126"/>
-      <c r="K26" s="126"/>
-      <c r="L26" s="126"/>
-      <c r="M26" s="126"/>
-      <c r="N26" s="126"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="20"/>
-      <c r="U26" s="20"/>
-      <c r="V26" s="20"/>
-      <c r="W26" s="20"/>
-    </row>
-    <row r="27" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="98" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="98"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="98"/>
-      <c r="F27" s="98"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="98"/>
-      <c r="I27" s="126"/>
-      <c r="J27" s="126"/>
-      <c r="K27" s="126"/>
-      <c r="L27" s="126"/>
-      <c r="M27" s="126"/>
-      <c r="N27" s="126"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-      <c r="T27" s="20"/>
-      <c r="U27" s="20"/>
-      <c r="V27" s="20"/>
-      <c r="W27" s="20"/>
-    </row>
-    <row r="28" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="111"/>
-      <c r="B28" s="99" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="99"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="113"/>
-      <c r="F28" s="99"/>
-      <c r="G28" s="99"/>
-      <c r="H28" s="99"/>
-      <c r="I28" s="127"/>
-      <c r="J28" s="127"/>
-      <c r="K28" s="127"/>
-      <c r="L28" s="127"/>
-      <c r="M28" s="127"/>
-      <c r="N28" s="127"/>
-      <c r="O28" s="111"/>
-      <c r="P28" s="111"/>
-      <c r="Q28" s="111"/>
-      <c r="R28" s="111"/>
-      <c r="S28" s="111"/>
-      <c r="T28" s="111"/>
-      <c r="U28" s="111"/>
-      <c r="V28" s="111"/>
-      <c r="W28" s="111"/>
-    </row>
-    <row r="29" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="111"/>
-      <c r="B29" s="99"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="127"/>
-      <c r="J29" s="127"/>
-      <c r="K29" s="127"/>
-      <c r="L29" s="127"/>
-      <c r="M29" s="127"/>
-      <c r="N29" s="127"/>
-      <c r="O29" s="111"/>
-      <c r="P29" s="111"/>
-      <c r="Q29" s="111"/>
-      <c r="R29" s="111"/>
-      <c r="S29" s="111"/>
-      <c r="T29" s="111"/>
-      <c r="U29" s="111"/>
-      <c r="V29" s="111"/>
-      <c r="W29" s="111"/>
-    </row>
-    <row r="30" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="111"/>
-      <c r="B30" s="99"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="99"/>
-      <c r="F30" s="99"/>
-      <c r="G30" s="99"/>
-      <c r="H30" s="99"/>
-      <c r="I30" s="127"/>
-      <c r="J30" s="127"/>
-      <c r="K30" s="127"/>
-      <c r="L30" s="127"/>
-      <c r="M30" s="127"/>
-      <c r="N30" s="127"/>
-      <c r="O30" s="111"/>
-      <c r="P30" s="111"/>
-      <c r="Q30" s="111"/>
-      <c r="R30" s="111"/>
-      <c r="S30" s="111"/>
-      <c r="T30" s="111"/>
-      <c r="U30" s="111"/>
-      <c r="V30" s="111"/>
-      <c r="W30" s="111"/>
-    </row>
-    <row r="31" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="111"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="99"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="99"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="127"/>
-      <c r="J31" s="127"/>
-      <c r="K31" s="127"/>
-      <c r="L31" s="127"/>
-      <c r="M31" s="127"/>
-      <c r="N31" s="127"/>
-      <c r="O31" s="111"/>
-      <c r="P31" s="111"/>
-      <c r="Q31" s="111"/>
-      <c r="R31" s="111"/>
-      <c r="S31" s="111"/>
-      <c r="T31" s="111"/>
-      <c r="U31" s="111"/>
-      <c r="V31" s="111"/>
-      <c r="W31" s="111"/>
-    </row>
-    <row r="32" spans="1:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="114"/>
-      <c r="B32" s="100"/>
-      <c r="C32" s="100"/>
-      <c r="D32" s="95"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="100"/>
-      <c r="G32" s="100"/>
-      <c r="H32" s="100"/>
-      <c r="I32" s="128"/>
-      <c r="J32" s="128"/>
-      <c r="K32" s="128"/>
-      <c r="L32" s="128"/>
-      <c r="M32" s="128"/>
-      <c r="N32" s="128"/>
-      <c r="O32" s="114"/>
-      <c r="P32" s="114"/>
-      <c r="Q32" s="114"/>
-      <c r="R32" s="114"/>
-      <c r="S32" s="114"/>
-      <c r="T32" s="114"/>
-      <c r="U32" s="114"/>
-      <c r="V32" s="114"/>
-      <c r="W32" s="114"/>
-    </row>
-    <row r="33" spans="1:23" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="96"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="96"/>
-      <c r="F33" s="96"/>
-      <c r="G33" s="96"/>
-      <c r="H33" s="96"/>
-      <c r="I33" s="129"/>
-      <c r="J33" s="129"/>
-      <c r="K33" s="129"/>
-      <c r="L33" s="129"/>
-      <c r="M33" s="129"/>
-      <c r="N33" s="129"/>
-    </row>
-    <row r="34" spans="1:23" s="20" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="133" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="115"/>
-      <c r="E34" s="115"/>
-      <c r="F34" s="115"/>
-      <c r="G34" s="115"/>
-      <c r="H34" s="115"/>
-      <c r="I34" s="130"/>
-      <c r="J34" s="126"/>
-      <c r="K34" s="126"/>
-      <c r="L34" s="126"/>
-      <c r="M34" s="126"/>
-      <c r="N34" s="126"/>
-    </row>
-    <row r="35" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" s="101"/>
-      <c r="F35" s="101"/>
-      <c r="G35" s="101"/>
-      <c r="H35" s="101"/>
-      <c r="I35" s="130"/>
-      <c r="J35" s="126"/>
-      <c r="K35" s="126"/>
-      <c r="L35" s="126"/>
-      <c r="M35" s="126"/>
-      <c r="N35" s="126"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="20"/>
-      <c r="Q35" s="20"/>
-      <c r="R35" s="20"/>
-      <c r="S35" s="20"/>
-      <c r="T35" s="20"/>
-      <c r="U35" s="20"/>
-      <c r="V35" s="20"/>
-      <c r="W35" s="20"/>
-    </row>
-    <row r="36" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="102" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="102"/>
-      <c r="F36" s="102"/>
-      <c r="G36" s="102"/>
-      <c r="H36" s="102"/>
-      <c r="I36" s="130"/>
-      <c r="J36" s="126"/>
-      <c r="K36" s="126"/>
-      <c r="L36" s="126"/>
-      <c r="M36" s="126"/>
-      <c r="N36" s="126"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="20"/>
-      <c r="R36" s="20"/>
-      <c r="S36" s="20"/>
-      <c r="T36" s="20"/>
-      <c r="U36" s="20"/>
-      <c r="V36" s="20"/>
-      <c r="W36" s="20"/>
-    </row>
-    <row r="37" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="111"/>
-      <c r="B37" s="103" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="116"/>
-      <c r="F37" s="103"/>
-      <c r="G37" s="103"/>
-      <c r="H37" s="103"/>
-      <c r="I37" s="131"/>
-      <c r="J37" s="127"/>
-      <c r="K37" s="127"/>
-      <c r="L37" s="127"/>
-      <c r="M37" s="127"/>
-      <c r="N37" s="127"/>
-      <c r="O37" s="111"/>
-      <c r="P37" s="111"/>
-      <c r="Q37" s="111"/>
-      <c r="R37" s="111"/>
-      <c r="S37" s="111"/>
-      <c r="T37" s="111"/>
-      <c r="U37" s="111"/>
-      <c r="V37" s="111"/>
-      <c r="W37" s="111"/>
-    </row>
-    <row r="38" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="111"/>
-      <c r="B38" s="103"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="103"/>
-      <c r="F38" s="103"/>
-      <c r="G38" s="103"/>
-      <c r="H38" s="103"/>
-      <c r="I38" s="131"/>
-      <c r="J38" s="127"/>
-      <c r="K38" s="127"/>
-      <c r="L38" s="127"/>
-      <c r="M38" s="127"/>
-      <c r="N38" s="127"/>
-      <c r="O38" s="111"/>
-      <c r="P38" s="111"/>
-      <c r="Q38" s="111"/>
-      <c r="R38" s="111"/>
-      <c r="S38" s="111"/>
-      <c r="T38" s="111"/>
-      <c r="U38" s="111"/>
-      <c r="V38" s="111"/>
-      <c r="W38" s="111"/>
-    </row>
-    <row r="39" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="111"/>
-      <c r="B39" s="103"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="103"/>
-      <c r="F39" s="103"/>
-      <c r="G39" s="103"/>
-      <c r="H39" s="103"/>
-      <c r="I39" s="131"/>
-      <c r="J39" s="127"/>
-      <c r="K39" s="127"/>
-      <c r="L39" s="127"/>
-      <c r="M39" s="127"/>
-      <c r="N39" s="127"/>
-      <c r="O39" s="111"/>
-      <c r="P39" s="111"/>
-      <c r="Q39" s="111"/>
-      <c r="R39" s="111"/>
-      <c r="S39" s="111"/>
-      <c r="T39" s="111"/>
-      <c r="U39" s="111"/>
-      <c r="V39" s="111"/>
-      <c r="W39" s="111"/>
-    </row>
-    <row r="40" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="111"/>
-      <c r="B40" s="103"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="103"/>
-      <c r="F40" s="103"/>
-      <c r="G40" s="103"/>
-      <c r="H40" s="103"/>
-      <c r="I40" s="131"/>
-      <c r="J40" s="127"/>
-      <c r="K40" s="127"/>
-      <c r="L40" s="127"/>
-      <c r="M40" s="127"/>
-      <c r="N40" s="127"/>
-      <c r="O40" s="111"/>
-      <c r="P40" s="111"/>
-      <c r="Q40" s="111"/>
-      <c r="R40" s="111"/>
-      <c r="S40" s="111"/>
-      <c r="T40" s="111"/>
-      <c r="U40" s="111"/>
-      <c r="V40" s="111"/>
-      <c r="W40" s="111"/>
-    </row>
-    <row r="41" spans="1:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="114"/>
-      <c r="B41" s="104"/>
-      <c r="C41" s="117"/>
-      <c r="D41" s="118"/>
-      <c r="E41" s="104"/>
-      <c r="F41" s="104"/>
-      <c r="G41" s="104"/>
-      <c r="H41" s="104"/>
-      <c r="I41" s="132"/>
-      <c r="J41" s="128"/>
-      <c r="K41" s="128"/>
-      <c r="L41" s="128"/>
-      <c r="M41" s="128"/>
-      <c r="N41" s="128"/>
-      <c r="O41" s="114"/>
-      <c r="P41" s="114"/>
-      <c r="Q41" s="114"/>
-      <c r="R41" s="114"/>
-      <c r="S41" s="114"/>
-      <c r="T41" s="114"/>
-      <c r="U41" s="114"/>
-      <c r="V41" s="114"/>
-      <c r="W41" s="114"/>
-    </row>
-    <row r="42" spans="1:23" s="20" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="133" t="s">
-        <v>59</v>
-      </c>
-      <c r="D42" s="109"/>
-      <c r="E42" s="115"/>
-      <c r="F42" s="115"/>
-      <c r="G42" s="115"/>
-      <c r="H42" s="115"/>
-      <c r="I42" s="130"/>
-      <c r="J42" s="126"/>
-      <c r="K42" s="126"/>
-      <c r="L42" s="126"/>
-      <c r="M42" s="126"/>
-      <c r="N42" s="126"/>
-    </row>
-    <row r="43" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="101" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="92" t="s">
-        <v>61</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E43" s="101"/>
-      <c r="F43" s="101"/>
-      <c r="G43" s="101"/>
-      <c r="H43" s="101"/>
-      <c r="I43" s="130"/>
-      <c r="J43" s="126"/>
-      <c r="K43" s="126"/>
-      <c r="L43" s="126"/>
-      <c r="M43" s="126"/>
-      <c r="N43" s="126"/>
-      <c r="O43" s="20"/>
-      <c r="P43" s="20"/>
-      <c r="Q43" s="20"/>
-      <c r="R43" s="20"/>
-      <c r="S43" s="20"/>
-      <c r="T43" s="20"/>
-      <c r="U43" s="20"/>
-      <c r="V43" s="20"/>
-      <c r="W43" s="20"/>
-    </row>
-    <row r="44" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="102" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="93" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="102"/>
-      <c r="F44" s="102"/>
-      <c r="G44" s="102"/>
-      <c r="H44" s="102"/>
-      <c r="I44" s="130"/>
-      <c r="J44" s="126"/>
-      <c r="K44" s="126"/>
-      <c r="L44" s="126"/>
-      <c r="M44" s="126"/>
-      <c r="N44" s="126"/>
-      <c r="O44" s="20"/>
-      <c r="P44" s="20"/>
-      <c r="Q44" s="20"/>
-      <c r="R44" s="20"/>
-      <c r="S44" s="20"/>
-      <c r="T44" s="20"/>
-      <c r="U44" s="20"/>
-      <c r="V44" s="20"/>
-      <c r="W44" s="20"/>
-    </row>
-    <row r="45" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="111"/>
-      <c r="B45" s="103" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="94" t="s">
+      <c r="D49" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E45" s="116"/>
-      <c r="F45" s="103"/>
-      <c r="G45" s="103"/>
-      <c r="H45" s="103"/>
-      <c r="I45" s="131"/>
-      <c r="J45" s="127"/>
-      <c r="K45" s="127"/>
-      <c r="L45" s="127"/>
-      <c r="M45" s="127"/>
-      <c r="N45" s="127"/>
-      <c r="O45" s="111"/>
-      <c r="P45" s="111"/>
-      <c r="Q45" s="111"/>
-      <c r="R45" s="111"/>
-      <c r="S45" s="111"/>
-      <c r="T45" s="111"/>
-      <c r="U45" s="111"/>
-      <c r="V45" s="111"/>
-      <c r="W45" s="111"/>
-    </row>
-    <row r="46" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="111"/>
-      <c r="B46" s="103"/>
-      <c r="C46" s="94"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="103"/>
-      <c r="F46" s="103"/>
-      <c r="G46" s="103"/>
-      <c r="H46" s="103"/>
-      <c r="I46" s="131"/>
-      <c r="J46" s="127"/>
-      <c r="K46" s="127"/>
-      <c r="L46" s="127"/>
-      <c r="M46" s="127"/>
-      <c r="N46" s="127"/>
-      <c r="O46" s="111"/>
-      <c r="P46" s="111"/>
-      <c r="Q46" s="111"/>
-      <c r="R46" s="111"/>
-      <c r="S46" s="111"/>
-      <c r="T46" s="111"/>
-      <c r="U46" s="111"/>
-      <c r="V46" s="111"/>
-      <c r="W46" s="111"/>
-    </row>
-    <row r="47" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="111"/>
-      <c r="B47" s="103"/>
-      <c r="C47" s="94"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="103"/>
-      <c r="F47" s="103"/>
-      <c r="G47" s="103"/>
-      <c r="H47" s="103"/>
-      <c r="I47" s="131"/>
-      <c r="J47" s="127"/>
-      <c r="K47" s="127"/>
-      <c r="L47" s="127"/>
-      <c r="M47" s="127"/>
-      <c r="N47" s="127"/>
-      <c r="O47" s="111"/>
-      <c r="P47" s="111"/>
-      <c r="Q47" s="111"/>
-      <c r="R47" s="111"/>
-      <c r="S47" s="111"/>
-      <c r="T47" s="111"/>
-      <c r="U47" s="111"/>
-      <c r="V47" s="111"/>
-      <c r="W47" s="111"/>
-    </row>
-    <row r="48" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="111"/>
-      <c r="B48" s="103"/>
-      <c r="C48" s="94"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="103"/>
-      <c r="F48" s="103"/>
-      <c r="G48" s="103"/>
-      <c r="H48" s="103"/>
-      <c r="I48" s="131"/>
-      <c r="J48" s="127"/>
-      <c r="K48" s="127"/>
-      <c r="L48" s="127"/>
-      <c r="M48" s="127"/>
-      <c r="N48" s="127"/>
-      <c r="O48" s="111"/>
-      <c r="P48" s="111"/>
-      <c r="Q48" s="111"/>
-      <c r="R48" s="111"/>
-      <c r="S48" s="111"/>
-      <c r="T48" s="111"/>
-      <c r="U48" s="111"/>
-      <c r="V48" s="111"/>
-      <c r="W48" s="111"/>
-    </row>
-    <row r="49" spans="1:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="114"/>
-      <c r="B49" s="104"/>
-      <c r="C49" s="119"/>
-      <c r="D49" s="118"/>
-      <c r="E49" s="104"/>
-      <c r="F49" s="104"/>
-      <c r="G49" s="104"/>
-      <c r="H49" s="104"/>
-      <c r="I49" s="132"/>
-      <c r="J49" s="128"/>
-      <c r="K49" s="128"/>
-      <c r="L49" s="128"/>
-      <c r="M49" s="128"/>
-      <c r="N49" s="128"/>
-      <c r="O49" s="114"/>
-      <c r="P49" s="114"/>
-      <c r="Q49" s="114"/>
-      <c r="R49" s="114"/>
-      <c r="S49" s="114"/>
-      <c r="T49" s="114"/>
-      <c r="U49" s="114"/>
-      <c r="V49" s="114"/>
-      <c r="W49" s="114"/>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C50" s="94"/>
-      <c r="D50" s="24"/>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E49" s="109"/>
+      <c r="F49" s="98"/>
+      <c r="G49" s="98"/>
+      <c r="H49" s="98"/>
+      <c r="I49" s="124"/>
+      <c r="J49" s="120"/>
+      <c r="K49" s="120"/>
+      <c r="L49" s="120"/>
+      <c r="M49" s="120"/>
+      <c r="N49" s="120"/>
+      <c r="O49" s="106"/>
+      <c r="P49" s="106"/>
+      <c r="Q49" s="106"/>
+      <c r="R49" s="106"/>
+      <c r="S49" s="106"/>
+      <c r="T49" s="106"/>
+      <c r="U49" s="106"/>
+      <c r="V49" s="106"/>
+      <c r="W49" s="106"/>
+    </row>
+    <row r="50" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="106"/>
+      <c r="B50" s="98"/>
+      <c r="C50" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E50" s="98"/>
+      <c r="F50" s="98"/>
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="124"/>
+      <c r="J50" s="120"/>
+      <c r="K50" s="120"/>
+      <c r="L50" s="120"/>
+      <c r="M50" s="120"/>
+      <c r="N50" s="120"/>
+      <c r="O50" s="106"/>
+      <c r="P50" s="106"/>
+      <c r="Q50" s="106"/>
+      <c r="R50" s="106"/>
+      <c r="S50" s="106"/>
+      <c r="T50" s="106"/>
+      <c r="U50" s="106"/>
+      <c r="V50" s="106"/>
+      <c r="W50" s="106"/>
+    </row>
+    <row r="51" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="106"/>
+      <c r="B51" s="98"/>
       <c r="C51" s="94"/>
       <c r="D51" s="24"/>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E51" s="98"/>
+      <c r="F51" s="98"/>
+      <c r="G51" s="98"/>
+      <c r="H51" s="98"/>
+      <c r="I51" s="124"/>
+      <c r="J51" s="120"/>
+      <c r="K51" s="120"/>
+      <c r="L51" s="120"/>
+      <c r="M51" s="120"/>
+      <c r="N51" s="120"/>
+      <c r="O51" s="106"/>
+      <c r="P51" s="106"/>
+      <c r="Q51" s="106"/>
+      <c r="R51" s="106"/>
+      <c r="S51" s="106"/>
+      <c r="T51" s="106"/>
+      <c r="U51" s="106"/>
+      <c r="V51" s="106"/>
+      <c r="W51" s="106"/>
+    </row>
+    <row r="52" spans="1:23" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="106"/>
+      <c r="B52" s="98"/>
+      <c r="C52" s="94"/>
       <c r="D52" s="24"/>
+      <c r="E52" s="98"/>
+      <c r="F52" s="98"/>
+      <c r="G52" s="98"/>
+      <c r="H52" s="98"/>
+      <c r="I52" s="124"/>
+      <c r="J52" s="120"/>
+      <c r="K52" s="120"/>
+      <c r="L52" s="120"/>
+      <c r="M52" s="120"/>
+      <c r="N52" s="120"/>
+      <c r="O52" s="106"/>
+      <c r="P52" s="106"/>
+      <c r="Q52" s="106"/>
+      <c r="R52" s="106"/>
+      <c r="S52" s="106"/>
+      <c r="T52" s="106"/>
+      <c r="U52" s="106"/>
+      <c r="V52" s="106"/>
+      <c r="W52" s="106"/>
+    </row>
+    <row r="53" spans="1:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="107"/>
+      <c r="B53" s="99"/>
+      <c r="C53" s="112"/>
+      <c r="D53" s="111"/>
+      <c r="E53" s="99"/>
+      <c r="F53" s="99"/>
+      <c r="G53" s="99"/>
+      <c r="H53" s="99"/>
+      <c r="I53" s="125"/>
+      <c r="J53" s="121"/>
+      <c r="K53" s="121"/>
+      <c r="L53" s="121"/>
+      <c r="M53" s="121"/>
+      <c r="N53" s="121"/>
+      <c r="O53" s="107"/>
+      <c r="P53" s="107"/>
+      <c r="Q53" s="107"/>
+      <c r="R53" s="107"/>
+      <c r="S53" s="107"/>
+      <c r="T53" s="107"/>
+      <c r="U53" s="107"/>
+      <c r="V53" s="107"/>
+      <c r="W53" s="107"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C54" s="94"/>
+      <c r="D54" s="24"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C55" s="94"/>
+      <c r="D55" s="24"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D56" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2744,8 +2891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2ABD43C-711F-4BD7-AEEF-0F35862BE21C}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0"/>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -2927,10 +3073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB080F3-0D40-4162-9445-826D86E6002D}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -2969,18 +3112,18 @@
     </row>
     <row r="2" spans="1:16" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D2" s="42"/>
       <c r="E2" s="42"/>
       <c r="F2" s="42"/>
       <c r="G2" s="42"/>
       <c r="H2" s="42" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I2" s="45"/>
       <c r="J2" s="42" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K2" s="48"/>
       <c r="L2" s="48"/>
@@ -2990,14 +3133,14 @@
       <c r="A3" s="46"/>
       <c r="B3" s="67"/>
       <c r="C3" s="71" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D3" s="72" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E3" s="72"/>
       <c r="F3" s="72"/>
-      <c r="G3" s="139"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="72"/>
       <c r="I3" s="45"/>
       <c r="J3" s="67"/>
@@ -3012,14 +3155,14 @@
       <c r="A4" s="46"/>
       <c r="B4" s="67"/>
       <c r="C4" s="73" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D4" s="74" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E4" s="74"/>
       <c r="F4" s="74"/>
-      <c r="G4" s="140"/>
+      <c r="G4" s="132"/>
       <c r="H4" s="74"/>
       <c r="I4" s="45"/>
       <c r="J4" s="67"/>
@@ -3036,7 +3179,7 @@
       <c r="D5" s="82"/>
       <c r="E5" s="83"/>
       <c r="F5" s="83"/>
-      <c r="G5" s="144"/>
+      <c r="G5" s="136"/>
       <c r="H5" s="83"/>
       <c r="I5" s="45"/>
       <c r="J5" s="67"/>
@@ -3048,7 +3191,7 @@
       <c r="D6" s="82"/>
       <c r="E6" s="83"/>
       <c r="F6" s="83"/>
-      <c r="G6" s="144"/>
+      <c r="G6" s="136"/>
       <c r="H6" s="83"/>
       <c r="I6" s="45"/>
       <c r="J6" s="67"/>
@@ -3060,7 +3203,7 @@
       <c r="D7" s="78"/>
       <c r="E7" s="79"/>
       <c r="F7" s="79"/>
-      <c r="G7" s="142"/>
+      <c r="G7" s="134"/>
       <c r="H7" s="79"/>
       <c r="I7" s="45"/>
       <c r="J7" s="63"/>
@@ -3072,7 +3215,7 @@
       <c r="D8" s="84"/>
       <c r="E8" s="69"/>
       <c r="F8" s="69"/>
-      <c r="G8" s="143"/>
+      <c r="G8" s="135"/>
       <c r="H8" s="69"/>
       <c r="I8" s="45"/>
       <c r="J8" s="63"/>
@@ -3081,7 +3224,7 @@
     <row r="9" spans="1:16" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="43" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D9" s="42"/>
       <c r="E9" s="42"/>
@@ -3090,7 +3233,7 @@
       <c r="H9" s="42"/>
       <c r="I9" s="45"/>
       <c r="J9" s="42" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K9" s="48"/>
       <c r="L9" s="48"/>
@@ -3100,16 +3243,16 @@
       <c r="A10" s="46"/>
       <c r="B10" s="67"/>
       <c r="C10" s="71" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E10" s="72"/>
       <c r="F10" s="72"/>
-      <c r="G10" s="139"/>
+      <c r="G10" s="131"/>
       <c r="H10" s="72" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I10" s="45"/>
       <c r="J10" s="67"/>
@@ -3124,16 +3267,16 @@
       <c r="A11" s="46"/>
       <c r="B11" s="67"/>
       <c r="C11" s="73" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D11" s="74" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E11" s="74"/>
       <c r="F11" s="74"/>
-      <c r="G11" s="140"/>
+      <c r="G11" s="132"/>
       <c r="H11" s="74" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I11" s="45"/>
       <c r="J11" s="67"/>
@@ -3151,7 +3294,7 @@
       <c r="D12" s="76"/>
       <c r="E12" s="76"/>
       <c r="F12" s="76"/>
-      <c r="G12" s="141"/>
+      <c r="G12" s="133"/>
       <c r="H12" s="76"/>
       <c r="I12" s="45"/>
       <c r="J12" s="67"/>
@@ -3168,7 +3311,7 @@
       <c r="D13" s="78"/>
       <c r="E13" s="79"/>
       <c r="F13" s="79"/>
-      <c r="G13" s="142"/>
+      <c r="G13" s="134"/>
       <c r="H13" s="79"/>
       <c r="J13" s="67"/>
       <c r="K13" s="68"/>
@@ -3179,7 +3322,7 @@
       <c r="D14" s="78"/>
       <c r="E14" s="79"/>
       <c r="F14" s="79"/>
-      <c r="G14" s="142"/>
+      <c r="G14" s="134"/>
       <c r="H14" s="79"/>
       <c r="J14" s="67"/>
       <c r="K14" s="68"/>
@@ -3190,7 +3333,7 @@
       <c r="D15" s="78"/>
       <c r="E15" s="79"/>
       <c r="F15" s="79"/>
-      <c r="G15" s="142"/>
+      <c r="G15" s="134"/>
       <c r="H15" s="79"/>
       <c r="J15" s="67"/>
       <c r="K15" s="68"/>
@@ -3201,7 +3344,7 @@
       <c r="D16" s="78"/>
       <c r="E16" s="79"/>
       <c r="F16" s="79"/>
-      <c r="G16" s="142"/>
+      <c r="G16" s="134"/>
       <c r="H16" s="79"/>
       <c r="J16" s="63"/>
       <c r="K16" s="68"/>
@@ -3211,13 +3354,13 @@
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="143"/>
+      <c r="G17" s="135"/>
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:16" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="C18" s="43" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D18" s="42"/>
       <c r="E18" s="42"/>
@@ -3225,7 +3368,7 @@
       <c r="G18" s="42"/>
       <c r="H18" s="42"/>
       <c r="J18" s="42" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K18" s="48"/>
       <c r="L18" s="48"/>
@@ -3238,7 +3381,7 @@
       <c r="D19" s="72"/>
       <c r="E19" s="72"/>
       <c r="F19" s="72"/>
-      <c r="G19" s="139"/>
+      <c r="G19" s="131"/>
       <c r="H19" s="72"/>
       <c r="I19" s="46"/>
       <c r="J19" s="67"/>
@@ -3256,7 +3399,7 @@
       <c r="D20" s="82"/>
       <c r="E20" s="82"/>
       <c r="F20" s="82"/>
-      <c r="G20" s="145"/>
+      <c r="G20" s="137"/>
       <c r="H20" s="82"/>
       <c r="I20" s="68"/>
       <c r="J20" s="87"/>
@@ -3272,7 +3415,7 @@
       <c r="D21" s="78"/>
       <c r="E21" s="78"/>
       <c r="F21" s="78"/>
-      <c r="G21" s="146"/>
+      <c r="G21" s="138"/>
       <c r="H21" s="78"/>
       <c r="I21" s="68"/>
       <c r="J21" s="68"/>
@@ -3282,7 +3425,7 @@
     <row r="22" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="40"/>
       <c r="C22" s="70"/>
-      <c r="G22" s="143"/>
+      <c r="G22" s="135"/>
     </row>
     <row r="23" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="40"/>
@@ -3360,10 +3503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D855BDC6-53B9-4E95-BC28-F624350AAB72}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58:D61"/>
-    </sheetView>
-    <sheetView topLeftCell="A9" workbookViewId="1">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>

</xml_diff>